<commit_message>
- Added seaonality to mosquito birth rate - Revised parameters - Initial setup of progbook
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_malaria.xlsx
+++ b/tests/databooks/databook_malaria.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -12,15 +12,17 @@
     <sheet name="Epidemic" sheetId="3" r:id="rId3"/>
     <sheet name="Cascade" sheetId="4" r:id="rId4"/>
     <sheet name="Mosquito properties" sheetId="5" r:id="rId5"/>
-    <sheet name="Interactions" sheetId="6" r:id="rId6"/>
-    <sheet name="Transfers" sheetId="7" r:id="rId7"/>
+    <sheet name="Constants" sheetId="8" r:id="rId6"/>
+    <sheet name="Seasonality" sheetId="9" r:id="rId7"/>
+    <sheet name="Interactions" sheetId="6" r:id="rId8"/>
+    <sheet name="Transfers" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="63">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -106,9 +108,6 @@
     <t>Mosquito prevalence</t>
   </si>
   <si>
-    <t>Number of bites per year per mosquito</t>
-  </si>
-  <si>
     <t>Incubation period (mosquito)</t>
   </si>
   <si>
@@ -173,6 +172,45 @@
   </si>
   <si>
     <t>Ageing</t>
+  </si>
+  <si>
+    <t>Factor to modify bites in human population</t>
+  </si>
+  <si>
+    <t>Factor to modify bites in human population (for nested programs)</t>
+  </si>
+  <si>
+    <t>Factor to modify bites in mosquito population</t>
+  </si>
+  <si>
+    <t>Factor to modify mosquito birth rate</t>
+  </si>
+  <si>
+    <t>Factor to modify mosquito life expectancy</t>
+  </si>
+  <si>
+    <t>Incubation period</t>
+  </si>
+  <si>
+    <t>Time to develop immunity</t>
+  </si>
+  <si>
+    <t>Duration of immunity</t>
+  </si>
+  <si>
+    <t>Time until immunity is lost</t>
+  </si>
+  <si>
+    <t>Treatment duration</t>
+  </si>
+  <si>
+    <t>Maximal mosquito birth rate</t>
+  </si>
+  <si>
+    <t>Minimal mosquito birth rate</t>
+  </si>
+  <si>
+    <t>Number of bites per time step per mosquito per human</t>
   </si>
 </sst>
 </file>
@@ -711,7 +749,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -790,6 +828,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -6770,34 +6835,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -7671,7 +7736,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:J23"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8505,7 +8570,7 @@
   <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27:J29"/>
+      <selection activeCell="Q27" sqref="Q27:V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10134,16 +10199,17 @@
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="15" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -10446,7 +10512,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -10497,8 +10563,8 @@
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="19">
-        <v>365</v>
+      <c r="C14" s="40">
+        <v>0.5</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>6</v>
@@ -10595,7 +10661,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
@@ -10744,7 +10810,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>3</v>
@@ -10893,7 +10959,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>3</v>
@@ -11312,6 +11378,1838 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O59"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="15" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29">
+        <v>2010</v>
+      </c>
+      <c r="F1" s="29">
+        <v>2011</v>
+      </c>
+      <c r="G1" s="29">
+        <v>2012</v>
+      </c>
+      <c r="H1" s="29">
+        <v>2013</v>
+      </c>
+      <c r="I1" s="29">
+        <v>2014</v>
+      </c>
+      <c r="J1" s="29">
+        <v>2015</v>
+      </c>
+      <c r="K1" s="29">
+        <v>2016</v>
+      </c>
+      <c r="L1" s="29">
+        <v>2017</v>
+      </c>
+      <c r="M1" s="29">
+        <v>2018</v>
+      </c>
+      <c r="N1" s="29">
+        <v>2019</v>
+      </c>
+      <c r="O1" s="29">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="31">
+        <v>1</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="31">
+        <v>1</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="31">
+        <v>1</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="31">
+        <v>1</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29">
+        <v>2010</v>
+      </c>
+      <c r="F7" s="29">
+        <v>2011</v>
+      </c>
+      <c r="G7" s="29">
+        <v>2012</v>
+      </c>
+      <c r="H7" s="29">
+        <v>2013</v>
+      </c>
+      <c r="I7" s="29">
+        <v>2014</v>
+      </c>
+      <c r="J7" s="29">
+        <v>2015</v>
+      </c>
+      <c r="K7" s="29">
+        <v>2016</v>
+      </c>
+      <c r="L7" s="29">
+        <v>2017</v>
+      </c>
+      <c r="M7" s="29">
+        <v>2018</v>
+      </c>
+      <c r="N7" s="29">
+        <v>2019</v>
+      </c>
+      <c r="O7" s="29">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="31">
+        <v>1</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="31">
+        <v>1</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="31">
+        <v>1</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="31">
+        <v>1</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29">
+        <v>2010</v>
+      </c>
+      <c r="F13" s="29">
+        <v>2011</v>
+      </c>
+      <c r="G13" s="29">
+        <v>2012</v>
+      </c>
+      <c r="H13" s="29">
+        <v>2013</v>
+      </c>
+      <c r="I13" s="29">
+        <v>2014</v>
+      </c>
+      <c r="J13" s="29">
+        <v>2015</v>
+      </c>
+      <c r="K13" s="29">
+        <v>2016</v>
+      </c>
+      <c r="L13" s="29">
+        <v>2017</v>
+      </c>
+      <c r="M13" s="29">
+        <v>2018</v>
+      </c>
+      <c r="N13" s="29">
+        <v>2019</v>
+      </c>
+      <c r="O13" s="29">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="31">
+        <v>1</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="31">
+        <v>1</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="31">
+        <v>1</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="31">
+        <v>1</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29">
+        <v>2010</v>
+      </c>
+      <c r="F19" s="29">
+        <v>2011</v>
+      </c>
+      <c r="G19" s="29">
+        <v>2012</v>
+      </c>
+      <c r="H19" s="29">
+        <v>2013</v>
+      </c>
+      <c r="I19" s="29">
+        <v>2014</v>
+      </c>
+      <c r="J19" s="29">
+        <v>2015</v>
+      </c>
+      <c r="K19" s="29">
+        <v>2016</v>
+      </c>
+      <c r="L19" s="29">
+        <v>2017</v>
+      </c>
+      <c r="M19" s="29">
+        <v>2018</v>
+      </c>
+      <c r="N19" s="29">
+        <v>2019</v>
+      </c>
+      <c r="O19" s="29">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="31">
+        <v>1</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="31">
+        <v>1</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="31">
+        <v>1</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="31">
+        <v>1</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="31"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29">
+        <v>2010</v>
+      </c>
+      <c r="F25" s="29">
+        <v>2011</v>
+      </c>
+      <c r="G25" s="29">
+        <v>2012</v>
+      </c>
+      <c r="H25" s="29">
+        <v>2013</v>
+      </c>
+      <c r="I25" s="29">
+        <v>2014</v>
+      </c>
+      <c r="J25" s="29">
+        <v>2015</v>
+      </c>
+      <c r="K25" s="29">
+        <v>2016</v>
+      </c>
+      <c r="L25" s="29">
+        <v>2017</v>
+      </c>
+      <c r="M25" s="29">
+        <v>2018</v>
+      </c>
+      <c r="N25" s="29">
+        <v>2019</v>
+      </c>
+      <c r="O25" s="29">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="29" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="31">
+        <v>1</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="29" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="31">
+        <v>1</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="31">
+        <v>1</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="31">
+        <v>1</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33">
+        <v>2010</v>
+      </c>
+      <c r="F31" s="33">
+        <v>2011</v>
+      </c>
+      <c r="G31" s="33">
+        <v>2012</v>
+      </c>
+      <c r="H31" s="33">
+        <v>2013</v>
+      </c>
+      <c r="I31" s="33">
+        <v>2014</v>
+      </c>
+      <c r="J31" s="33">
+        <v>2015</v>
+      </c>
+      <c r="K31" s="33">
+        <v>2016</v>
+      </c>
+      <c r="L31" s="33">
+        <v>2017</v>
+      </c>
+      <c r="M31" s="33">
+        <v>2018</v>
+      </c>
+      <c r="N31" s="33">
+        <v>2019</v>
+      </c>
+      <c r="O31" s="33">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="35">
+        <v>3.8356164383561653E-2</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="35"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="35">
+        <v>3.8356164383561653E-2</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="35"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B34" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="35">
+        <v>3.8356164383561653E-2</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="35"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="35">
+        <v>3.8356164383561653E-2</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="35"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33">
+        <v>2010</v>
+      </c>
+      <c r="F37" s="33">
+        <v>2011</v>
+      </c>
+      <c r="G37" s="33">
+        <v>2012</v>
+      </c>
+      <c r="H37" s="33">
+        <v>2013</v>
+      </c>
+      <c r="I37" s="33">
+        <v>2014</v>
+      </c>
+      <c r="J37" s="33">
+        <v>2015</v>
+      </c>
+      <c r="K37" s="33">
+        <v>2016</v>
+      </c>
+      <c r="L37" s="33">
+        <v>2017</v>
+      </c>
+      <c r="M37" s="33">
+        <v>2018</v>
+      </c>
+      <c r="N37" s="33">
+        <v>2019</v>
+      </c>
+      <c r="O37" s="33">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="35">
+        <v>2.7397260273972601E-2</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="35"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="35"/>
+      <c r="N38" s="35"/>
+      <c r="O38" s="35"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="35">
+        <v>2.7397260273972601E-2</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="35"/>
+      <c r="L39" s="35"/>
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="35"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B40" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="35">
+        <v>2.7397260273972601E-2</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="35">
+        <v>2.7397260273972601E-2</v>
+      </c>
+      <c r="D41" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="35"/>
+      <c r="L41" s="35"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33">
+        <v>2010</v>
+      </c>
+      <c r="F43" s="33">
+        <v>2011</v>
+      </c>
+      <c r="G43" s="33">
+        <v>2012</v>
+      </c>
+      <c r="H43" s="33">
+        <v>2013</v>
+      </c>
+      <c r="I43" s="33">
+        <v>2014</v>
+      </c>
+      <c r="J43" s="33">
+        <v>2015</v>
+      </c>
+      <c r="K43" s="33">
+        <v>2016</v>
+      </c>
+      <c r="L43" s="33">
+        <v>2017</v>
+      </c>
+      <c r="M43" s="33">
+        <v>2018</v>
+      </c>
+      <c r="N43" s="33">
+        <v>2019</v>
+      </c>
+      <c r="O43" s="33">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="35">
+        <v>8.2191780821917804E-2</v>
+      </c>
+      <c r="D44" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="35"/>
+      <c r="M44" s="35"/>
+      <c r="N44" s="35"/>
+      <c r="O44" s="35"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B45" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="35">
+        <v>8.2191780821917804E-2</v>
+      </c>
+      <c r="D45" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="35"/>
+      <c r="M45" s="35"/>
+      <c r="N45" s="35"/>
+      <c r="O45" s="35"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B46" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="35">
+        <v>8.2191780821917804E-2</v>
+      </c>
+      <c r="D46" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="35"/>
+      <c r="N46" s="35"/>
+      <c r="O46" s="35"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B47" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="35">
+        <v>8.2191780821917804E-2</v>
+      </c>
+      <c r="D47" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="35"/>
+      <c r="L47" s="35"/>
+      <c r="M47" s="35"/>
+      <c r="N47" s="35"/>
+      <c r="O47" s="35"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33">
+        <v>2010</v>
+      </c>
+      <c r="F49" s="33">
+        <v>2011</v>
+      </c>
+      <c r="G49" s="33">
+        <v>2012</v>
+      </c>
+      <c r="H49" s="33">
+        <v>2013</v>
+      </c>
+      <c r="I49" s="33">
+        <v>2014</v>
+      </c>
+      <c r="J49" s="33">
+        <v>2015</v>
+      </c>
+      <c r="K49" s="33">
+        <v>2016</v>
+      </c>
+      <c r="L49" s="33">
+        <v>2017</v>
+      </c>
+      <c r="M49" s="33">
+        <v>2018</v>
+      </c>
+      <c r="N49" s="33">
+        <v>2019</v>
+      </c>
+      <c r="O49" s="33">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B50" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="35">
+        <v>0.24657534246575341</v>
+      </c>
+      <c r="D50" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="35"/>
+      <c r="L50" s="35"/>
+      <c r="M50" s="35"/>
+      <c r="N50" s="35"/>
+      <c r="O50" s="35"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="33" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B51" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="35">
+        <v>0.24657534246575341</v>
+      </c>
+      <c r="D51" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="35"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="35"/>
+      <c r="L51" s="35"/>
+      <c r="M51" s="35"/>
+      <c r="N51" s="35"/>
+      <c r="O51" s="35"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B52" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="35">
+        <v>0.24657534246575341</v>
+      </c>
+      <c r="D52" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="35"/>
+      <c r="L52" s="35"/>
+      <c r="M52" s="35"/>
+      <c r="N52" s="35"/>
+      <c r="O52" s="35"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B53" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="35">
+        <v>0.24657534246575341</v>
+      </c>
+      <c r="D53" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="35"/>
+      <c r="L53" s="35"/>
+      <c r="M53" s="35"/>
+      <c r="N53" s="35"/>
+      <c r="O53" s="35"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="33"/>
+      <c r="E55" s="33">
+        <v>2010</v>
+      </c>
+      <c r="F55" s="33">
+        <v>2011</v>
+      </c>
+      <c r="G55" s="33">
+        <v>2012</v>
+      </c>
+      <c r="H55" s="33">
+        <v>2013</v>
+      </c>
+      <c r="I55" s="33">
+        <v>2014</v>
+      </c>
+      <c r="J55" s="33">
+        <v>2015</v>
+      </c>
+      <c r="K55" s="33">
+        <v>2016</v>
+      </c>
+      <c r="L55" s="33">
+        <v>2017</v>
+      </c>
+      <c r="M55" s="33">
+        <v>2018</v>
+      </c>
+      <c r="N55" s="33">
+        <v>2019</v>
+      </c>
+      <c r="O55" s="33">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B56" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="35">
+        <v>5.4794520547945202E-2</v>
+      </c>
+      <c r="D56" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="35"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="35"/>
+      <c r="I56" s="35"/>
+      <c r="J56" s="35"/>
+      <c r="K56" s="35"/>
+      <c r="L56" s="35"/>
+      <c r="M56" s="35"/>
+      <c r="N56" s="35"/>
+      <c r="O56" s="35"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B57" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="35">
+        <v>5.4794520547945202E-2</v>
+      </c>
+      <c r="D57" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="35"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="35"/>
+      <c r="H57" s="35"/>
+      <c r="I57" s="35"/>
+      <c r="J57" s="35"/>
+      <c r="K57" s="35"/>
+      <c r="L57" s="35"/>
+      <c r="M57" s="35"/>
+      <c r="N57" s="35"/>
+      <c r="O57" s="35"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B58" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="35">
+        <v>5.4794520547945202E-2</v>
+      </c>
+      <c r="D58" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="35"/>
+      <c r="H58" s="35"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="35"/>
+      <c r="L58" s="35"/>
+      <c r="M58" s="35"/>
+      <c r="N58" s="35"/>
+      <c r="O58" s="35"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="33" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B59" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="35">
+        <v>5.4794520547945202E-2</v>
+      </c>
+      <c r="D59" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="35"/>
+      <c r="H59" s="35"/>
+      <c r="I59" s="35"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="35"/>
+      <c r="L59" s="35"/>
+      <c r="M59" s="35"/>
+      <c r="N59" s="35"/>
+      <c r="O59" s="35"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="15" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37">
+        <v>2010</v>
+      </c>
+      <c r="F1" s="37">
+        <v>2011</v>
+      </c>
+      <c r="G1" s="37">
+        <v>2012</v>
+      </c>
+      <c r="H1" s="37">
+        <v>2013</v>
+      </c>
+      <c r="I1" s="37">
+        <v>2014</v>
+      </c>
+      <c r="J1" s="37">
+        <v>2015</v>
+      </c>
+      <c r="K1" s="37">
+        <v>2016</v>
+      </c>
+      <c r="L1" s="37">
+        <v>2017</v>
+      </c>
+      <c r="M1" s="37">
+        <v>2018</v>
+      </c>
+      <c r="N1" s="37">
+        <v>2019</v>
+      </c>
+      <c r="O1" s="37">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="39">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="39">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="39">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="39">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37">
+        <v>2010</v>
+      </c>
+      <c r="F7" s="37">
+        <v>2011</v>
+      </c>
+      <c r="G7" s="37">
+        <v>2012</v>
+      </c>
+      <c r="H7" s="37">
+        <v>2013</v>
+      </c>
+      <c r="I7" s="37">
+        <v>2014</v>
+      </c>
+      <c r="J7" s="37">
+        <v>2015</v>
+      </c>
+      <c r="K7" s="37">
+        <v>2016</v>
+      </c>
+      <c r="L7" s="37">
+        <v>2017</v>
+      </c>
+      <c r="M7" s="37">
+        <v>2018</v>
+      </c>
+      <c r="N7" s="37">
+        <v>2019</v>
+      </c>
+      <c r="O7" s="37">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="39">
+        <v>0.9</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="39">
+        <v>0.9</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="39">
+        <v>0.9</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="39">
+        <v>0.9</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF808080"/>
@@ -11340,10 +13238,10 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -11370,16 +13268,16 @@
         <v>mos</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -11388,16 +13286,16 @@
         <v>gp</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -11406,16 +13304,16 @@
         <v>preg</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -11424,16 +13322,16 @@
         <v>child</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -11495,7 +13393,7 @@
         <v>...</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="4">
         <v>1</v>
@@ -11530,7 +13428,7 @@
         <v>...</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
@@ -11565,7 +13463,7 @@
         <v>...</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="4">
         <v>1</v>
@@ -11600,7 +13498,7 @@
         <v>...</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="4">
         <v>1</v>
@@ -11635,7 +13533,7 @@
         <v>mos</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="4">
         <v>1</v>
@@ -11670,7 +13568,7 @@
         <v>...</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -11705,7 +13603,7 @@
         <v>...</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17" s="4">
         <v>1</v>
@@ -11740,7 +13638,7 @@
         <v>...</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18" s="4">
         <v>1</v>
@@ -11775,7 +13673,7 @@
         <v>mos</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19" s="4">
         <v>1</v>
@@ -11810,7 +13708,7 @@
         <v>...</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" s="4">
         <v>1</v>
@@ -11845,7 +13743,7 @@
         <v>...</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E21" s="4">
         <v>1</v>
@@ -11880,7 +13778,7 @@
         <v>...</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="4">
         <v>1</v>
@@ -11915,7 +13813,7 @@
         <v>mos</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E23" s="4">
         <v>1</v>
@@ -11950,7 +13848,7 @@
         <v>...</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24" s="4">
         <v>1</v>
@@ -11985,7 +13883,7 @@
         <v>...</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E25" s="4">
         <v>1</v>
@@ -12020,7 +13918,7 @@
         <v>...</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26" s="4">
         <v>1</v>
@@ -12051,10 +13949,10 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
         <v>36</v>
-      </c>
-      <c r="B29" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -12081,16 +13979,16 @@
         <v>mos</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -12099,16 +13997,16 @@
         <v>gp</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -12117,16 +14015,16 @@
         <v>preg</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -12135,16 +14033,16 @@
         <v>child</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -12206,7 +14104,7 @@
         <v>...</v>
       </c>
       <c r="D38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E38" s="4">
         <v>1</v>
@@ -12241,7 +14139,7 @@
         <v>...</v>
       </c>
       <c r="D39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E39" s="4">
         <v>1</v>
@@ -12276,7 +14174,7 @@
         <v>...</v>
       </c>
       <c r="D40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E40" s="4">
         <v>1</v>
@@ -12311,7 +14209,7 @@
         <v>...</v>
       </c>
       <c r="D41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E41" s="4">
         <v>1</v>
@@ -12346,7 +14244,7 @@
         <v>mos</v>
       </c>
       <c r="D42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E42" s="4">
         <v>0.5</v>
@@ -12381,7 +14279,7 @@
         <v>...</v>
       </c>
       <c r="D43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E43" s="4">
         <v>1</v>
@@ -12416,7 +14314,7 @@
         <v>...</v>
       </c>
       <c r="D44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E44" s="4">
         <v>1</v>
@@ -12451,7 +14349,7 @@
         <v>...</v>
       </c>
       <c r="D45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E45" s="4">
         <v>1</v>
@@ -12486,7 +14384,7 @@
         <v>mos</v>
       </c>
       <c r="D46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E46" s="4">
         <v>0.3</v>
@@ -12521,7 +14419,7 @@
         <v>...</v>
       </c>
       <c r="D47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E47" s="4">
         <v>1</v>
@@ -12556,7 +14454,7 @@
         <v>...</v>
       </c>
       <c r="D48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E48" s="4">
         <v>1</v>
@@ -12591,7 +14489,7 @@
         <v>...</v>
       </c>
       <c r="D49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E49" s="4">
         <v>1</v>
@@ -12626,7 +14524,7 @@
         <v>mos</v>
       </c>
       <c r="D50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E50" s="4">
         <v>0.2</v>
@@ -12661,7 +14559,7 @@
         <v>...</v>
       </c>
       <c r="D51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E51" s="4">
         <v>1</v>
@@ -12696,7 +14594,7 @@
         <v>...</v>
       </c>
       <c r="D52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E52" s="4">
         <v>1</v>
@@ -12731,7 +14629,7 @@
         <v>...</v>
       </c>
       <c r="D53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E53" s="4">
         <v>1</v>
@@ -12762,10 +14660,10 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>37</v>
+      </c>
+      <c r="B56" t="s">
         <v>38</v>
-      </c>
-      <c r="B56" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
@@ -12792,16 +14690,16 @@
         <v>mos</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E59" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
@@ -12810,16 +14708,16 @@
         <v>gp</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D60" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E60" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
@@ -12828,16 +14726,16 @@
         <v>preg</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D61" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E61" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
@@ -12846,16 +14744,16 @@
         <v>child</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D62" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E62" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
@@ -12917,7 +14815,7 @@
         <v>...</v>
       </c>
       <c r="D65" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E65" s="4">
         <v>1</v>
@@ -12952,7 +14850,7 @@
         <v>gp</v>
       </c>
       <c r="D66" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E66" s="4">
         <v>1</v>
@@ -12987,7 +14885,7 @@
         <v>preg</v>
       </c>
       <c r="D67" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E67" s="4">
         <v>1</v>
@@ -13022,7 +14920,7 @@
         <v>child</v>
       </c>
       <c r="D68" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E68" s="4">
         <v>1</v>
@@ -13057,7 +14955,7 @@
         <v>...</v>
       </c>
       <c r="D69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E69" s="4">
         <v>1</v>
@@ -13092,7 +14990,7 @@
         <v>gp</v>
       </c>
       <c r="D70" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E70" s="4">
         <v>1</v>
@@ -13127,7 +15025,7 @@
         <v>preg</v>
       </c>
       <c r="D71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E71" s="4">
         <v>1</v>
@@ -13162,7 +15060,7 @@
         <v>child</v>
       </c>
       <c r="D72" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E72" s="4">
         <v>1</v>
@@ -13197,7 +15095,7 @@
         <v>...</v>
       </c>
       <c r="D73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E73" s="4">
         <v>1</v>
@@ -13232,7 +15130,7 @@
         <v>gp</v>
       </c>
       <c r="D74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E74" s="4">
         <v>1</v>
@@ -13267,7 +15165,7 @@
         <v>preg</v>
       </c>
       <c r="D75" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E75" s="4">
         <v>1</v>
@@ -13302,7 +15200,7 @@
         <v>child</v>
       </c>
       <c r="D76" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E76" s="4">
         <v>1</v>
@@ -13337,7 +15235,7 @@
         <v>...</v>
       </c>
       <c r="D77" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E77" s="4">
         <v>1</v>
@@ -13372,7 +15270,7 @@
         <v>gp</v>
       </c>
       <c r="D78" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E78" s="4">
         <v>1</v>
@@ -13407,7 +15305,7 @@
         <v>preg</v>
       </c>
       <c r="D79" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E79" s="4">
         <v>1</v>
@@ -13442,7 +15340,7 @@
         <v>child</v>
       </c>
       <c r="D80" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E80" s="4">
         <v>1</v>
@@ -14976,15 +16874,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF808080"/>
   </sheetPr>
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15005,10 +16903,10 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -15035,16 +16933,16 @@
         <v>mos</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -15053,16 +16951,16 @@
         <v>gp</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -15071,16 +16969,16 @@
         <v>preg</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -15089,16 +16987,16 @@
         <v>child</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
initial implemenatation of accumulated DALYs
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_malaria.xlsx
+++ b/tests/databooks/databook_malaria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -14,15 +14,16 @@
     <sheet name="Mosquito properties" sheetId="5" r:id="rId5"/>
     <sheet name="Constants" sheetId="8" r:id="rId6"/>
     <sheet name="Seasonality" sheetId="9" r:id="rId7"/>
-    <sheet name="Interactions" sheetId="6" r:id="rId8"/>
-    <sheet name="Transfers" sheetId="7" r:id="rId9"/>
+    <sheet name="DALYs" sheetId="10" r:id="rId8"/>
+    <sheet name="Interactions" sheetId="6" r:id="rId9"/>
+    <sheet name="Transfers" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="65">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -211,6 +212,12 @@
   </si>
   <si>
     <t>Number of bites per time step per mosquito per human</t>
+  </si>
+  <si>
+    <t>Disability weight</t>
+  </si>
+  <si>
+    <t>Average years lost due to premature death</t>
   </si>
 </sst>
 </file>
@@ -6870,6 +6877,1130 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF808080"/>
+  </sheetPr>
+  <dimension ref="A1:Q26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
+        <v>2010</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2011</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2012</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2013</v>
+      </c>
+      <c r="K10" s="1">
+        <v>2014</v>
+      </c>
+      <c r="L10" s="1">
+        <v>2015</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2016</v>
+      </c>
+      <c r="N10" s="1">
+        <v>2017</v>
+      </c>
+      <c r="O10" s="1">
+        <v>2018</v>
+      </c>
+      <c r="P10" s="1">
+        <v>2019</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="str">
+        <f>IF($B$5="Y",'Population Definitions'!$A$2,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B11" s="3" t="str">
+        <f>IF($B$5="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>IF($B$5="Y",'Population Definitions'!$A$2,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3" t="str">
+        <f>IF($B$5="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <f>IF($C$5="Y",'Population Definitions'!$A$2,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B12" s="3" t="str">
+        <f>IF($C$5="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>IF($C$5="Y",'Population Definitions'!$A$3,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3" t="str">
+        <f>IF($C$5="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="str">
+        <f>IF($D$5="Y",'Population Definitions'!$A$2,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B13" s="3" t="str">
+        <f>IF($D$5="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>IF($D$5="Y",'Population Definitions'!$A$4,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3" t="str">
+        <f>IF($D$5="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
+        <f>IF($E$5="Y",'Population Definitions'!$A$2,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B14" s="3" t="str">
+        <f>IF($E$5="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>IF($E$5="Y",'Population Definitions'!$A$5,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3" t="str">
+        <f>IF($E$5="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="str">
+        <f>IF($B$6="Y",'Population Definitions'!$A$3,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B15" s="3" t="str">
+        <f>IF($B$6="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f>IF($B$6="Y",'Population Definitions'!$A$2,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3" t="str">
+        <f>IF($B$6="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="str">
+        <f>IF($C$6="Y",'Population Definitions'!$A$3,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B16" s="3" t="str">
+        <f>IF($C$6="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f>IF($C$6="Y",'Population Definitions'!$A$3,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3" t="str">
+        <f>IF($C$6="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="str">
+        <f>IF($D$6="Y",'Population Definitions'!$A$3,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B17" s="3" t="str">
+        <f>IF($D$6="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f>IF($D$6="Y",'Population Definitions'!$A$4,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3" t="str">
+        <f>IF($D$6="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="str">
+        <f>IF($E$6="Y",'Population Definitions'!$A$3,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B18" s="3" t="str">
+        <f>IF($E$6="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f>IF($E$6="Y",'Population Definitions'!$A$5,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3" t="str">
+        <f>IF($E$6="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="str">
+        <f>IF($B$7="Y",'Population Definitions'!$A$4,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B19" s="3" t="str">
+        <f>IF($B$7="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <f>IF($B$7="Y",'Population Definitions'!$A$2,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3" t="str">
+        <f>IF($B$7="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="str">
+        <f>IF($C$7="Y",'Population Definitions'!$A$4,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B20" s="3" t="str">
+        <f>IF($C$7="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f>IF($C$7="Y",'Population Definitions'!$A$3,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3" t="str">
+        <f>IF($C$7="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="str">
+        <f>IF($D$7="Y",'Population Definitions'!$A$4,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B21" s="3" t="str">
+        <f>IF($D$7="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f>IF($D$7="Y",'Population Definitions'!$A$4,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="3" t="str">
+        <f>IF($D$7="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="str">
+        <f>IF($E$7="Y",'Population Definitions'!$A$4,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B22" s="3" t="str">
+        <f>IF($E$7="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <f>IF($E$7="Y",'Population Definitions'!$A$5,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="3" t="str">
+        <f>IF($E$7="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="str">
+        <f>IF($B$8="Y",'Population Definitions'!$A$5,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B23" s="3" t="str">
+        <f>IF($B$8="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <f>IF($B$8="Y",'Population Definitions'!$A$2,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="3" t="str">
+        <f>IF($B$8="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="str">
+        <f>IF($C$8="Y",'Population Definitions'!$A$5,"...")</f>
+        <v>child</v>
+      </c>
+      <c r="B24" s="3" t="str">
+        <f>IF($C$8="Y","---&gt;","...")</f>
+        <v>---&gt;</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <f>IF($C$8="Y",'Population Definitions'!$A$3,"...")</f>
+        <v>gp</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="F24" s="3" t="str">
+        <f>IF($C$8="Y","OR","...")</f>
+        <v>OR</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="str">
+        <f>IF($D$8="Y",'Population Definitions'!$A$5,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B25" s="3" t="str">
+        <f>IF($D$8="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f>IF($D$8="Y",'Population Definitions'!$A$4,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="3" t="str">
+        <f>IF($D$8="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="str">
+        <f>IF($E$8="Y",'Population Definitions'!$A$5,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="B26" s="3" t="str">
+        <f>IF($E$8="Y","---&gt;","...")</f>
+        <v>...</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <f>IF($E$8="Y",'Population Definitions'!$A$5,"...")</f>
+        <v>...</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="3" t="str">
+        <f>IF($E$8="Y","OR","...")</f>
+        <v>...</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="cellIs" dxfId="87" priority="7" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="8" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="cellIs" dxfId="85" priority="13" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="14" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="cellIs" dxfId="83" priority="19" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="20" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="cellIs" dxfId="81" priority="1" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="2" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="cellIs" dxfId="79" priority="15" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="16" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="77" priority="21" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="22" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="cellIs" dxfId="75" priority="3" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="4" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="73" priority="9" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="10" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="cellIs" dxfId="71" priority="23" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="24" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="expression" dxfId="69" priority="25">
+      <formula>COUNTIF(G11:Q11,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="26">
+      <formula>AND(COUNTIF(G11:Q11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E11)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="27">
+      <formula>$B$5&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="expression" dxfId="66" priority="29">
+      <formula>COUNTIF(G12:Q12,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="30">
+      <formula>AND(COUNTIF(G12:Q12,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E12)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="31">
+      <formula>$C$5&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="expression" dxfId="63" priority="33">
+      <formula>COUNTIF(G13:Q13,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="34">
+      <formula>AND(COUNTIF(G13:Q13,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E13)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="35">
+      <formula>$D$5&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="expression" dxfId="60" priority="37">
+      <formula>COUNTIF(G14:Q14,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="38">
+      <formula>AND(COUNTIF(G14:Q14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E14)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="39">
+      <formula>$E$5&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="expression" dxfId="57" priority="41">
+      <formula>COUNTIF(G15:Q15,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="42">
+      <formula>AND(COUNTIF(G15:Q15,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E15)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="43">
+      <formula>$B$6&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="expression" dxfId="54" priority="45">
+      <formula>COUNTIF(G16:Q16,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="46">
+      <formula>AND(COUNTIF(G16:Q16,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E16)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="47">
+      <formula>$C$6&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="expression" dxfId="51" priority="49">
+      <formula>COUNTIF(G17:Q17,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="50">
+      <formula>AND(COUNTIF(G17:Q17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E17)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="51">
+      <formula>$D$6&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="expression" dxfId="48" priority="53">
+      <formula>COUNTIF(G18:Q18,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="54">
+      <formula>AND(COUNTIF(G18:Q18,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E18)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="55">
+      <formula>$E$6&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="expression" dxfId="45" priority="57">
+      <formula>COUNTIF(G19:Q19,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="58">
+      <formula>AND(COUNTIF(G19:Q19,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E19)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="59">
+      <formula>$B$7&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="expression" dxfId="42" priority="61">
+      <formula>COUNTIF(G20:Q20,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="62">
+      <formula>AND(COUNTIF(G20:Q20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E20)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="63">
+      <formula>$C$7&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="expression" dxfId="39" priority="65">
+      <formula>COUNTIF(G21:Q21,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="66">
+      <formula>AND(COUNTIF(G21:Q21,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E21)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="67">
+      <formula>$D$7&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="expression" dxfId="36" priority="69">
+      <formula>COUNTIF(G22:Q22,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="70">
+      <formula>AND(COUNTIF(G22:Q22,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E22)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="71">
+      <formula>$E$7&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="expression" dxfId="33" priority="73">
+      <formula>COUNTIF(G23:Q23,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="74">
+      <formula>AND(COUNTIF(G23:Q23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E23)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="75">
+      <formula>$B$8&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="expression" dxfId="30" priority="77">
+      <formula>COUNTIF(G24:Q24,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="78">
+      <formula>AND(COUNTIF(G24:Q24,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E24)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="79">
+      <formula>$C$8&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="expression" dxfId="27" priority="81">
+      <formula>COUNTIF(G25:Q25,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="82">
+      <formula>AND(COUNTIF(G25:Q25,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E25)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="83">
+      <formula>$D$8&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="expression" dxfId="24" priority="85">
+      <formula>COUNTIF(G26:Q26,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="86">
+      <formula>AND(COUNTIF(G26:Q26,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E26)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="87">
+      <formula>$E$8&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:Q11">
+    <cfRule type="expression" dxfId="15" priority="28">
+      <formula>$B$5&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:Q12">
+    <cfRule type="expression" dxfId="14" priority="32">
+      <formula>$C$5&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:Q13">
+    <cfRule type="expression" dxfId="13" priority="36">
+      <formula>$D$5&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14:Q14">
+    <cfRule type="expression" dxfId="12" priority="40">
+      <formula>$E$5&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15:Q15">
+    <cfRule type="expression" dxfId="11" priority="44">
+      <formula>$B$6&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16:Q16">
+    <cfRule type="expression" dxfId="10" priority="48">
+      <formula>$C$6&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17:Q17">
+    <cfRule type="expression" dxfId="9" priority="52">
+      <formula>$D$6&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18:Q18">
+    <cfRule type="expression" dxfId="8" priority="56">
+      <formula>$E$6&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G19:Q19">
+    <cfRule type="expression" dxfId="7" priority="60">
+      <formula>$B$7&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20:Q20">
+    <cfRule type="expression" dxfId="6" priority="64">
+      <formula>$C$7&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G21:Q21">
+    <cfRule type="expression" dxfId="5" priority="68">
+      <formula>$D$7&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22:Q22">
+    <cfRule type="expression" dxfId="4" priority="72">
+      <formula>$E$7&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23:Q23">
+    <cfRule type="expression" dxfId="3" priority="76">
+      <formula>$B$8&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24:Q24">
+    <cfRule type="expression" dxfId="2" priority="80">
+      <formula>$C$8&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25:Q25">
+    <cfRule type="expression" dxfId="1" priority="84">
+      <formula>$D$8&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26:Q26">
+    <cfRule type="expression" dxfId="0" priority="88">
+      <formula>$E$8&lt;&gt;"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"N.A."</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
+      <formula1>"N.A."</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7">
+      <formula1>"N.A."</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8">
+      <formula1>"N.A."</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D21">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D22">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D26">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C5" location="Transfers!C12" display="N"/>
+    <hyperlink ref="D5" location="Transfers!C13" display="N"/>
+    <hyperlink ref="E5" location="Transfers!C14" display="N"/>
+    <hyperlink ref="B6" location="Transfers!C15" display="N"/>
+    <hyperlink ref="D6" location="Transfers!C17" display="N"/>
+    <hyperlink ref="E6" location="Transfers!C18" display="N"/>
+    <hyperlink ref="B7" location="Transfers!C19" display="N"/>
+    <hyperlink ref="C7" location="Transfers!C20" display="N"/>
+    <hyperlink ref="E7" location="Transfers!C22" display="N"/>
+    <hyperlink ref="B8" location="Transfers!C23" display="N"/>
+    <hyperlink ref="C8" location="Transfers!C24" display="N"/>
+    <hyperlink ref="D8" location="Transfers!C25" display="N"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
@@ -10199,7 +11330,7 @@
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -11382,7 +12513,7 @@
   <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12894,7 +14025,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13210,6 +14341,343 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="15" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37">
+        <v>2010</v>
+      </c>
+      <c r="F1" s="37">
+        <v>2011</v>
+      </c>
+      <c r="G1" s="37">
+        <v>2012</v>
+      </c>
+      <c r="H1" s="37">
+        <v>2013</v>
+      </c>
+      <c r="I1" s="37">
+        <v>2014</v>
+      </c>
+      <c r="J1" s="37">
+        <v>2015</v>
+      </c>
+      <c r="K1" s="37">
+        <v>2016</v>
+      </c>
+      <c r="L1" s="37">
+        <v>2017</v>
+      </c>
+      <c r="M1" s="37">
+        <v>2018</v>
+      </c>
+      <c r="N1" s="37">
+        <v>2019</v>
+      </c>
+      <c r="O1" s="37">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="39">
+        <v>0</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="39">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="39">
+        <v>0.62280000000000002</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="39">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37">
+        <v>2010</v>
+      </c>
+      <c r="F7" s="37">
+        <v>2011</v>
+      </c>
+      <c r="G7" s="37">
+        <v>2012</v>
+      </c>
+      <c r="H7" s="37">
+        <v>2013</v>
+      </c>
+      <c r="I7" s="37">
+        <v>2014</v>
+      </c>
+      <c r="J7" s="37">
+        <v>2015</v>
+      </c>
+      <c r="K7" s="37">
+        <v>2016</v>
+      </c>
+      <c r="L7" s="37">
+        <v>2017</v>
+      </c>
+      <c r="M7" s="37">
+        <v>2018</v>
+      </c>
+      <c r="N7" s="37">
+        <v>2019</v>
+      </c>
+      <c r="O7" s="37">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mos</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="39">
+        <v>0</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="str">
+        <f>'Population Definitions'!$A$3</f>
+        <v>gp</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="39">
+        <v>27.89</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="str">
+        <f>'Population Definitions'!$A$4</f>
+        <v>preg</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="39">
+        <v>28.06</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="str">
+        <f>'Population Definitions'!$A$5</f>
+        <v>child</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="39">
+        <v>30.77</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF808080"/>
@@ -16872,1128 +18340,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF808080"/>
-  </sheetPr>
-  <dimension ref="A1:Q26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="str">
-        <f>'Population Definitions'!$A$2</f>
-        <v>mos</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <f>'Population Definitions'!$A$3</f>
-        <v>gp</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f>'Population Definitions'!$A$4</f>
-        <v>preg</v>
-      </c>
-      <c r="E4" s="1" t="str">
-        <f>'Population Definitions'!$A$5</f>
-        <v>child</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="str">
-        <f>'Population Definitions'!$A$2</f>
-        <v>mos</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="str">
-        <f>'Population Definitions'!$A$3</f>
-        <v>gp</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="str">
-        <f>'Population Definitions'!$A$4</f>
-        <v>preg</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="str">
-        <f>'Population Definitions'!$A$5</f>
-        <v>child</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1">
-        <v>2010</v>
-      </c>
-      <c r="H10" s="1">
-        <v>2011</v>
-      </c>
-      <c r="I10" s="1">
-        <v>2012</v>
-      </c>
-      <c r="J10" s="1">
-        <v>2013</v>
-      </c>
-      <c r="K10" s="1">
-        <v>2014</v>
-      </c>
-      <c r="L10" s="1">
-        <v>2015</v>
-      </c>
-      <c r="M10" s="1">
-        <v>2016</v>
-      </c>
-      <c r="N10" s="1">
-        <v>2017</v>
-      </c>
-      <c r="O10" s="1">
-        <v>2018</v>
-      </c>
-      <c r="P10" s="1">
-        <v>2019</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="str">
-        <f>IF($B$5="Y",'Population Definitions'!$A$2,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B11" s="3" t="str">
-        <f>IF($B$5="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C11" s="1" t="str">
-        <f>IF($B$5="Y",'Population Definitions'!$A$2,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3" t="str">
-        <f>IF($B$5="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="str">
-        <f>IF($C$5="Y",'Population Definitions'!$A$2,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B12" s="3" t="str">
-        <f>IF($C$5="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C12" s="1" t="str">
-        <f>IF($C$5="Y",'Population Definitions'!$A$3,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3" t="str">
-        <f>IF($C$5="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="str">
-        <f>IF($D$5="Y",'Population Definitions'!$A$2,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B13" s="3" t="str">
-        <f>IF($D$5="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C13" s="1" t="str">
-        <f>IF($D$5="Y",'Population Definitions'!$A$4,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3" t="str">
-        <f>IF($D$5="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="str">
-        <f>IF($E$5="Y",'Population Definitions'!$A$2,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B14" s="3" t="str">
-        <f>IF($E$5="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C14" s="1" t="str">
-        <f>IF($E$5="Y",'Population Definitions'!$A$5,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3" t="str">
-        <f>IF($E$5="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="str">
-        <f>IF($B$6="Y",'Population Definitions'!$A$3,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B15" s="3" t="str">
-        <f>IF($B$6="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C15" s="1" t="str">
-        <f>IF($B$6="Y",'Population Definitions'!$A$2,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3" t="str">
-        <f>IF($B$6="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="str">
-        <f>IF($C$6="Y",'Population Definitions'!$A$3,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B16" s="3" t="str">
-        <f>IF($C$6="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C16" s="1" t="str">
-        <f>IF($C$6="Y",'Population Definitions'!$A$3,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="3" t="str">
-        <f>IF($C$6="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="str">
-        <f>IF($D$6="Y",'Population Definitions'!$A$3,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B17" s="3" t="str">
-        <f>IF($D$6="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C17" s="1" t="str">
-        <f>IF($D$6="Y",'Population Definitions'!$A$4,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3" t="str">
-        <f>IF($D$6="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="str">
-        <f>IF($E$6="Y",'Population Definitions'!$A$3,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B18" s="3" t="str">
-        <f>IF($E$6="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C18" s="1" t="str">
-        <f>IF($E$6="Y",'Population Definitions'!$A$5,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3" t="str">
-        <f>IF($E$6="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="str">
-        <f>IF($B$7="Y",'Population Definitions'!$A$4,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B19" s="3" t="str">
-        <f>IF($B$7="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C19" s="1" t="str">
-        <f>IF($B$7="Y",'Population Definitions'!$A$2,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3" t="str">
-        <f>IF($B$7="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="str">
-        <f>IF($C$7="Y",'Population Definitions'!$A$4,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B20" s="3" t="str">
-        <f>IF($C$7="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C20" s="1" t="str">
-        <f>IF($C$7="Y",'Population Definitions'!$A$3,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3" t="str">
-        <f>IF($C$7="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="str">
-        <f>IF($D$7="Y",'Population Definitions'!$A$4,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B21" s="3" t="str">
-        <f>IF($D$7="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C21" s="1" t="str">
-        <f>IF($D$7="Y",'Population Definitions'!$A$4,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3" t="str">
-        <f>IF($D$7="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="str">
-        <f>IF($E$7="Y",'Population Definitions'!$A$4,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B22" s="3" t="str">
-        <f>IF($E$7="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C22" s="1" t="str">
-        <f>IF($E$7="Y",'Population Definitions'!$A$5,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="3" t="str">
-        <f>IF($E$7="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="str">
-        <f>IF($B$8="Y",'Population Definitions'!$A$5,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B23" s="3" t="str">
-        <f>IF($B$8="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C23" s="1" t="str">
-        <f>IF($B$8="Y",'Population Definitions'!$A$2,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="3" t="str">
-        <f>IF($B$8="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="str">
-        <f>IF($C$8="Y",'Population Definitions'!$A$5,"...")</f>
-        <v>child</v>
-      </c>
-      <c r="B24" s="3" t="str">
-        <f>IF($C$8="Y","---&gt;","...")</f>
-        <v>---&gt;</v>
-      </c>
-      <c r="C24" s="1" t="str">
-        <f>IF($C$8="Y",'Population Definitions'!$A$3,"...")</f>
-        <v>gp</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="27">
-        <v>0.2</v>
-      </c>
-      <c r="F24" s="3" t="str">
-        <f>IF($C$8="Y","OR","...")</f>
-        <v>OR</v>
-      </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="str">
-        <f>IF($D$8="Y",'Population Definitions'!$A$5,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B25" s="3" t="str">
-        <f>IF($D$8="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C25" s="1" t="str">
-        <f>IF($D$8="Y",'Population Definitions'!$A$4,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="3" t="str">
-        <f>IF($D$8="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="str">
-        <f>IF($E$8="Y",'Population Definitions'!$A$5,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="B26" s="3" t="str">
-        <f>IF($E$8="Y","---&gt;","...")</f>
-        <v>...</v>
-      </c>
-      <c r="C26" s="1" t="str">
-        <f>IF($E$8="Y",'Population Definitions'!$A$5,"...")</f>
-        <v>...</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="3" t="str">
-        <f>IF($E$8="Y","OR","...")</f>
-        <v>...</v>
-      </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="87" priority="7" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="8" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="85" priority="13" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="14" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" dxfId="83" priority="19" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="20" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="81" priority="1" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="2" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="79" priority="15" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="16" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="77" priority="21" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="22" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="75" priority="3" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="4" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="73" priority="9" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="10" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="71" priority="23" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="24" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="69" priority="25">
-      <formula>COUNTIF(G11:Q11,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="68" priority="26">
-      <formula>AND(COUNTIF(G11:Q11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E11)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="27">
-      <formula>$B$5&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="expression" dxfId="66" priority="29">
-      <formula>COUNTIF(G12:Q12,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="30">
-      <formula>AND(COUNTIF(G12:Q12,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E12)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="31">
-      <formula>$C$5&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="63" priority="33">
-      <formula>COUNTIF(G13:Q13,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="34">
-      <formula>AND(COUNTIF(G13:Q13,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E13)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="61" priority="35">
-      <formula>$D$5&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="60" priority="37">
-      <formula>COUNTIF(G14:Q14,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="38">
-      <formula>AND(COUNTIF(G14:Q14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E14)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="39">
-      <formula>$E$5&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="57" priority="41">
-      <formula>COUNTIF(G15:Q15,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="42">
-      <formula>AND(COUNTIF(G15:Q15,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E15)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="55" priority="43">
-      <formula>$B$6&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
-    <cfRule type="expression" dxfId="54" priority="45">
-      <formula>COUNTIF(G16:Q16,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="53" priority="46">
-      <formula>AND(COUNTIF(G16:Q16,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E16)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="47">
-      <formula>$C$6&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="expression" dxfId="51" priority="49">
-      <formula>COUNTIF(G17:Q17,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="50" priority="50">
-      <formula>AND(COUNTIF(G17:Q17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E17)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="49" priority="51">
-      <formula>$D$6&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="expression" dxfId="48" priority="53">
-      <formula>COUNTIF(G18:Q18,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="54">
-      <formula>AND(COUNTIF(G18:Q18,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E18)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="55">
-      <formula>$E$6&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="45" priority="57">
-      <formula>COUNTIF(G19:Q19,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="58">
-      <formula>AND(COUNTIF(G19:Q19,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E19)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="59">
-      <formula>$B$7&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
-    <cfRule type="expression" dxfId="42" priority="61">
-      <formula>COUNTIF(G20:Q20,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="62">
-      <formula>AND(COUNTIF(G20:Q20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E20)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="63">
-      <formula>$C$7&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="expression" dxfId="39" priority="65">
-      <formula>COUNTIF(G21:Q21,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="66">
-      <formula>AND(COUNTIF(G21:Q21,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E21)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="67">
-      <formula>$D$7&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="expression" dxfId="36" priority="69">
-      <formula>COUNTIF(G22:Q22,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="70">
-      <formula>AND(COUNTIF(G22:Q22,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E22)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="71">
-      <formula>$E$7&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="expression" dxfId="33" priority="73">
-      <formula>COUNTIF(G23:Q23,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="74">
-      <formula>AND(COUNTIF(G23:Q23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E23)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="31" priority="75">
-      <formula>$B$8&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="30" priority="77">
-      <formula>COUNTIF(G24:Q24,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="78">
-      <formula>AND(COUNTIF(G24:Q24,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E24)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="79">
-      <formula>$C$8&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="expression" dxfId="27" priority="81">
-      <formula>COUNTIF(G25:Q25,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="82">
-      <formula>AND(COUNTIF(G25:Q25,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E25)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="83">
-      <formula>$D$8&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26">
-    <cfRule type="expression" dxfId="24" priority="85">
-      <formula>COUNTIF(G26:Q26,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="86">
-      <formula>AND(COUNTIF(G26:Q26,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E26)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="87">
-      <formula>$E$8&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G11:Q11">
-    <cfRule type="expression" dxfId="15" priority="28">
-      <formula>$B$5&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12:Q12">
-    <cfRule type="expression" dxfId="14" priority="32">
-      <formula>$C$5&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G13:Q13">
-    <cfRule type="expression" dxfId="13" priority="36">
-      <formula>$D$5&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G14:Q14">
-    <cfRule type="expression" dxfId="12" priority="40">
-      <formula>$E$5&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G15:Q15">
-    <cfRule type="expression" dxfId="11" priority="44">
-      <formula>$B$6&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G16:Q16">
-    <cfRule type="expression" dxfId="10" priority="48">
-      <formula>$C$6&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G17:Q17">
-    <cfRule type="expression" dxfId="9" priority="52">
-      <formula>$D$6&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G18:Q18">
-    <cfRule type="expression" dxfId="8" priority="56">
-      <formula>$E$6&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G19:Q19">
-    <cfRule type="expression" dxfId="7" priority="60">
-      <formula>$B$7&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G20:Q20">
-    <cfRule type="expression" dxfId="6" priority="64">
-      <formula>$C$7&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G21:Q21">
-    <cfRule type="expression" dxfId="5" priority="68">
-      <formula>$D$7&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G22:Q22">
-    <cfRule type="expression" dxfId="4" priority="72">
-      <formula>$E$7&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G23:Q23">
-    <cfRule type="expression" dxfId="3" priority="76">
-      <formula>$B$8&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G24:Q24">
-    <cfRule type="expression" dxfId="2" priority="80">
-      <formula>$C$8&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G25:Q25">
-    <cfRule type="expression" dxfId="1" priority="84">
-      <formula>$D$8&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G26:Q26">
-    <cfRule type="expression" dxfId="0" priority="88">
-      <formula>$E$8&lt;&gt;"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="32">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"N.A."</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
-      <formula1>"N.A."</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7">
-      <formula1>"N.A."</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8">
-      <formula1>"N.A."</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D21">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D22">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D26">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C5" location="Transfers!C12" display="N"/>
-    <hyperlink ref="D5" location="Transfers!C13" display="N"/>
-    <hyperlink ref="E5" location="Transfers!C14" display="N"/>
-    <hyperlink ref="B6" location="Transfers!C15" display="N"/>
-    <hyperlink ref="D6" location="Transfers!C17" display="N"/>
-    <hyperlink ref="E6" location="Transfers!C18" display="N"/>
-    <hyperlink ref="B7" location="Transfers!C19" display="N"/>
-    <hyperlink ref="C7" location="Transfers!C20" display="N"/>
-    <hyperlink ref="E7" location="Transfers!C22" display="N"/>
-    <hyperlink ref="B8" location="Transfers!C23" display="N"/>
-    <hyperlink ref="C8" location="Transfers!C24" display="N"/>
-    <hyperlink ref="D8" location="Transfers!C25" display="N"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>